<commit_message>
deleted .idea file in webpage add, maintanince to the repo, changed plans excel file
</commit_message>
<xml_diff>
--- a/Documentation/plans.xlsx
+++ b/Documentation/plans.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshb\Desktop\Evil stuff\GrizzlyHacks\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7197CEF-977A-482C-AD43-9AA4B3F782CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766C155-6D6D-409A-AFB7-47F1F97E2BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17112" windowHeight="8808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,19 +27,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>get code base up</t>
+    <t>create home page</t>
   </si>
   <si>
-    <t>choose which version of angular to use</t>
+    <t>login stuff</t>
   </si>
   <si>
-    <t>create basic layout</t>
+    <t>user dashboard</t>
   </si>
   <si>
-    <t>design basic structure of database</t>
+    <t>admin dashboard</t>
   </si>
   <si>
-    <t>design system</t>
+    <t>event calander</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>